<commit_message>
Resolved classroom scheduling conflicts
</commit_message>
<xml_diff>
--- a/backend/output_timetables/Faculty_Availability_Schedule_Audit.xlsx
+++ b/backend/output_timetables/Faculty_Availability_Schedule_Audit.xlsx
@@ -530,10 +530,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="60" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
     <col width="60" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="60" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -622,9 +622,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E3" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec B [C004]</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -644,9 +644,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Post-Mid) | DSAI [L403]</t>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -683,7 +683,7 @@
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec B [C003]</t>
+          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec A [C004]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -735,19 +735,19 @@
           <t>15:30-17:00</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Post-Mid) | DSAI [L403]</t>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec B [C003]</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec A [C004]</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec B [C004]</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -845,11 +845,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="57" customWidth="1" min="2" max="2"/>
+    <col width="48" customWidth="1" min="2" max="2"/>
     <col width="57" customWidth="1" min="3" max="3"/>
     <col width="57" customWidth="1" min="4" max="4"/>
-    <col width="55" customWidth="1" min="5" max="5"/>
-    <col width="55" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -927,24 +927,24 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t>MA162 (Probability) Sem 1 (Pre-Mid) | DSAI [C001]</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
-        </is>
-      </c>
-      <c r="E3" s="5" t="inlineStr">
-        <is>
-          <t>MA263 (Random Processes) Sem 3 (Pre-Mid) | ECE [L405]</t>
-        </is>
-      </c>
-      <c r="F3" s="5" t="inlineStr">
-        <is>
-          <t>MA263 (Random Processes) Sem 3 (Pre-Mid) | ECE [L405]</t>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>MA263 (Random Processes) Sem 3 (Pre-Mid) | ECE</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
     </row>
@@ -956,17 +956,17 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>MA162 (Probability) Sem 1 (Pre-Mid) | DSAI [C001]</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+          <t>MA263 (Random Processes) Sem 3 (Pre-Mid) | ECE</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec B [C004]</t>
         </is>
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec A [C001]</t>
+          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec A [C004]</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -986,19 +986,20 @@
           <t>13:00-14:30</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec B [C001]</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec A [C001]</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec B [C004]
+MA162 (Probability) Sem 1 (Pre-Mid) | ECE [C002]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -1057,7 +1058,8 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec B [C001]</t>
+          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec A [C004]
+MA162 (Probability) Sem 1 (Pre-Mid) | ECE [C002]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -1161,10 +1163,10 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="56" customWidth="1" min="2" max="2"/>
-    <col width="56" customWidth="1" min="3" max="3"/>
-    <col width="57" customWidth="1" min="4" max="4"/>
-    <col width="57" customWidth="1" min="5" max="5"/>
-    <col width="57" customWidth="1" min="6" max="6"/>
+    <col width="49" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1254,10 +1256,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C002]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L403]</t>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -1282,10 +1283,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [L403]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L404]</t>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -1315,10 +1315,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L407]
-CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [L408]</t>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -1340,8 +1339,8 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE [C102]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE [C203]</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE [C302]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE [C101]</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -1376,10 +1375,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L406]
-CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI</t>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -1392,10 +1390,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C002]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L207]</t>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
     </row>
@@ -1425,10 +1422,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="F8" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C002]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L207]</t>
+      <c r="F8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
     </row>
@@ -1661,8 +1657,8 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [C304]
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [C305]</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [L402]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [C205]</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -1709,7 +1705,7 @@
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [L107]
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B
 CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B</t>
         </is>
       </c>
@@ -1742,8 +1738,8 @@
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [L107]
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [L208]</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [C001]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [C101]</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -1804,7 +1800,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="60" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
     <col width="60" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
@@ -1918,10 +1914,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [L408]
-CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI</t>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D4" s="5" t="inlineStr">
@@ -2018,14 +2013,13 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B [L402]
-CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec B [L404]</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [C102]
-CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C104]</t>
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B [C203]
+CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec B [C305]</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -2045,16 +2039,15 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="B8" s="5" t="inlineStr">
-        <is>
-          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [C104]
-CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C205]</t>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B [C203]
-CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec B [C302]</t>
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B [C104]
+CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec B [C204]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -2126,8 +2119,8 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
@@ -2276,9 +2269,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>DS161 (Introduction to DATA science and artificial intelligence) Sem 1 (Post-Mid) | ECE [C002]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -2335,9 +2328,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>DS161 (Introduction to DATA science and artificial intelligence) Sem 1 (Post-Mid) | ECE [C002]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -2686,8 +2679,8 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>EC351 (Introduction to Algorithms) Sem 5 (Pre-Mid) | ECE [L404]
-EC351 (Introduction to Algorithms) Sem 5 (Post-Mid) | ECE [L408]</t>
+          <t>EC351 (Introduction to Algorithms) Sem 5 (Pre-Mid) | ECE [L408]
+EC351 (Introduction to Algorithms) Sem 5 (Post-Mid) | ECE [C305]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -2935,7 +2928,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>EC301 (Introduction to VLSI Design) Sem 5 (Pre-Mid) | ECE [L405]
+          <t>EC301 (Introduction to VLSI Design) Sem 5 (Pre-Mid) | ECE [L404]
 EC301 (Introduction to VLSI Design) Sem 5 (Post-Mid) | ECE [L403]</t>
         </is>
       </c>
@@ -3190,16 +3183,15 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [L408]
-CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A [L408]
 CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec A</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -3257,9 +3249,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec A [L405]</t>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -3289,15 +3281,14 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A [L408]</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [C102]
-CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C104]</t>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -3317,15 +3308,15 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="B8" s="5" t="inlineStr">
-        <is>
-          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [C104]
-CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C205]</t>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A [C204]</t>
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A [C203]
+CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec A [C202]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -3396,7 +3387,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="60" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
     <col width="60" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
@@ -3480,13 +3471,14 @@
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [C304]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [C002]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [C102]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [C305]</t>
         </is>
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [C004]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L403]</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -3602,15 +3594,15 @@
           <t>15:30-17:00</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L408]</t>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L107]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L207]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L106]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -3642,8 +3634,8 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L107]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [C004]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L207]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L106]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -4118,18 +4110,18 @@
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | ECE [C001]
-MA261 (Differential Equations) Sem 3 (Post-Mid) | DSAI [L408]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | DSAI [L407]
+MA261 (Differential Equations) Sem 3 (Post-Mid) | DSAI [L407]</t>
         </is>
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec A [L407]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec A [C001]</t>
         </is>
       </c>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec A [L407]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec A [C001]</t>
         </is>
       </c>
     </row>
@@ -4156,7 +4148,7 @@
       </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | ECE [C001]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec B [C001]</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -4178,13 +4170,13 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec B [L407]
-MA261 (Differential Equations) Sem 3 (Post-Mid) | DSAI [L408]</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec B [C001]
+MA261 (Differential Equations) Sem 3 (Post-Mid) | DSAI [L407]</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [C303]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -4211,7 +4203,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | ECE [C001]</t>
+          <t>MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [L407]</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -4243,7 +4235,8 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | DSAI [L408]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | DSAI [C001]
+MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [L407]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -4346,8 +4339,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="55" customWidth="1" min="2" max="2"/>
+    <col width="55" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
@@ -4428,9 +4421,10 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [C302]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE [C303]</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -4455,9 +4449,10 @@
           <t>10:30-12:00</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [C205]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE [C302]</t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
@@ -4487,9 +4482,10 @@
           <t>13:00-14:30</t>
         </is>
       </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE
+CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -4519,9 +4515,10 @@
           <t>14:30-15:30</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [L208]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE [L208]</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -4662,10 +4659,10 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="53" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
     <col width="60" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="60" customWidth="1" min="6" max="6"/>
+    <col width="60" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4775,19 +4772,19 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE</t>
-        </is>
-      </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [L406]</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [C302]</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -4812,9 +4809,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [L408]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -4881,14 +4878,14 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E7" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
-        </is>
-      </c>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [C004]</t>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [L105]</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
     </row>
@@ -4913,14 +4910,14 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E8" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
-        </is>
-      </c>
-      <c r="F8" s="5" t="inlineStr">
-        <is>
-          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [C004]</t>
+      <c r="E8" s="5" t="inlineStr">
+        <is>
+          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [L105]</t>
+        </is>
+      </c>
+      <c r="F8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
     </row>
@@ -5217,8 +5214,8 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec B [C304]
-CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec B [C003]</t>
+          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec B [C305]
+CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec B [C002]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -5383,14 +5380,14 @@
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [L402]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [L405]</t>
         </is>
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [C302]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [C304]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [C104]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [C302]</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -5410,9 +5407,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C002]</t>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -5445,7 +5442,7 @@
       <c r="C5" s="5" t="inlineStr">
         <is>
           <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C204]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [C205]</t>
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C205]</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -5482,14 +5479,14 @@
       </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C101]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C102]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C102]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C203]</t>
         </is>
       </c>
       <c r="E6" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [C101]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [C104]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [C102]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [C101]</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
@@ -5516,7 +5513,8 @@
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C101]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C104]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C202]</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -5614,11 +5612,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="54" customWidth="1" min="2" max="2"/>
+    <col width="60" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
     <col width="60" customWidth="1" min="4" max="4"/>
     <col width="60" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="53" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5708,12 +5706,13 @@
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [C004]</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [C004]
+EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [C102]</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [C004]</t>
         </is>
       </c>
     </row>
@@ -5728,14 +5727,14 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>EC161 (Digital Design) Sem 1 (Pre-Mid) | DSAI [C003]</t>
-        </is>
-      </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [C001]</t>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -5762,17 +5761,18 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Pre-Mid) | DSAI [L105]</t>
-        </is>
-      </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [C001]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [C004]</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E5" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [L206]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [L105]
+EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
@@ -5792,9 +5792,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>EC161 (Digital Design) Sem 1 (Pre-Mid) | DSAI [L105]</t>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -5804,7 +5804,8 @@
       </c>
       <c r="E6" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [L206]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [L105]
+EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [C004]</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
@@ -5821,22 +5822,22 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Pre-Mid) | DSAI [C003]</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [C001]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [C004]</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [L206]</t>
-        </is>
-      </c>
-      <c r="E7" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [C004]</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [L206]</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
@@ -5861,14 +5862,14 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [L206]</t>
-        </is>
-      </c>
-      <c r="E8" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="E8" s="5" t="inlineStr">
+        <is>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [L206]</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -6045,8 +6046,8 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [C102]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [L402]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [C205]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [C305]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -6137,8 +6138,8 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [L406]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [L402]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [L403]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -6181,8 +6182,8 @@
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [C101]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [C102]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [C002]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [C001]</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -6785,7 +6786,7 @@
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE</t>
+          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE [C002]</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
@@ -6817,7 +6818,7 @@
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE [C003]</t>
+          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE [C002]</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -6880,7 +6881,7 @@
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="60" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="60" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
@@ -6960,9 +6961,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t>HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec B [C202]</t>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -6987,20 +6988,21 @@
           <t>10:30-12:00</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec B [C202]</t>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec B [C203]
-HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec A [C204]</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec A [C101]
+HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec A [C104]</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec B [C101]
+HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec B [C104]</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -7025,9 +7027,10 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec B [C101]
+HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec B [C102]</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -7086,8 +7089,8 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec B [C203]
-HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec A [C204]</t>
+          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec A [C101]
+HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec A [C102]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -7195,11 +7198,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="51" customWidth="1" min="2" max="2"/>
+    <col width="55" customWidth="1" min="2" max="2"/>
     <col width="55" customWidth="1" min="3" max="3"/>
     <col width="55" customWidth="1" min="4" max="4"/>
     <col width="60" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="60" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7309,19 +7312,20 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec B [C004]</t>
         </is>
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec B [C003]</t>
-        </is>
-      </c>
-      <c r="E4" s="5" t="inlineStr">
-        <is>
-          <t>DA261 (Statistical Programming) Sem 3 (Post-Mid) | DSAI [C104]</t>
+          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec A [C004]
+MA161 (Statistics) Sem 1 (Post-Mid) | ECE [C101]</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -7336,15 +7340,15 @@
           <t>13:00-14:30</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>MA161 (Statistics) Sem 1 (Post-Mid) | DSAI [L404]</t>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec B [C003]
-MA161 (Statistics) Sem 1 (Post-Mid) | DSAI [L404]</t>
+          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec A [C004]
+MA161 (Statistics) Sem 1 (Post-Mid) | ECE [C101]</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -7384,9 +7388,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E6" s="5" t="inlineStr">
-        <is>
-          <t>DA261 (Statistical Programming) Sem 3 (Post-Mid) | DSAI [L407]</t>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
@@ -7401,9 +7405,9 @@
           <t>15:30-17:00</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec B [C004]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -7421,9 +7425,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="F7" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>DA261 (Statistical Programming) Sem 3 (Post-Mid) | DSAI [L403]</t>
         </is>
       </c>
     </row>
@@ -7453,9 +7457,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="F8" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="F8" s="5" t="inlineStr">
+        <is>
+          <t>DA261 (Statistical Programming) Sem 3 (Post-Mid) | DSAI [L403]</t>
         </is>
       </c>
     </row>
@@ -7514,7 +7518,7 @@
     <col width="60" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="60" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -7627,9 +7631,10 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [L403]
+CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [L404]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -7637,9 +7642,10 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [L402]
+CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C205]</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -7750,15 +7756,16 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [C104]
+CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C205]</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>DS303 (Algorithms and Data Structures) Sem 5 (Pre-Mid) | DSAI [L406]
-DS303 (Algorithms and Data Structures) Sem 5 (Post-Mid) | DSAI [C305]</t>
+          <t>DS303 (Algorithms and Data Structures) Sem 5 (Pre-Mid) | DSAI [C303]
+DS303 (Algorithms and Data Structures) Sem 5 (Post-Mid) | DSAI [C304]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -8683,7 +8690,7 @@
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [C303]
+          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI
 DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI</t>
         </is>
       </c>
@@ -8701,8 +8708,8 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [L403]
-DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [L404]</t>
+          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [C003]
+DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [C004]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -8717,8 +8724,8 @@
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [C303]
-DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [C002]</t>
+          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [C205]
+DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [C104]</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -8988,8 +8995,8 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>EC306 (Digital Signal Processing) Sem 5 (Pre-Mid) | ECE [L206]
-EC306 (Digital Signal Processing) Sem 5 (Post-Mid) | ECE [L105]</t>
+          <t>EC306 (Digital Signal Processing) Sem 5 (Pre-Mid) | ECE [L105]
+EC306 (Digital Signal Processing) Sem 5 (Post-Mid) | ECE [L206]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -9021,8 +9028,8 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>EC306 (Digital Signal Processing) Sem 5 (Pre-Mid) | ECE [L206]
-EC306 (Digital Signal Processing) Sem 5 (Post-Mid) | ECE [L105]</t>
+          <t>EC306 (Digital Signal Processing) Sem 5 (Pre-Mid) | ECE [L105]
+EC306 (Digital Signal Processing) Sem 5 (Post-Mid) | ECE [L206]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -9098,8 +9105,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="56" customWidth="1" min="2" max="2"/>
-    <col width="56" customWidth="1" min="3" max="3"/>
+    <col width="54" customWidth="1" min="2" max="2"/>
+    <col width="54" customWidth="1" min="3" max="3"/>
     <col width="57" customWidth="1" min="4" max="4"/>
     <col width="57" customWidth="1" min="5" max="5"/>
     <col width="57" customWidth="1" min="6" max="6"/>
@@ -9177,25 +9184,26 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE
-CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE</t>
+          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L406]
+DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L408]</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE
-CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L404]
+DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L406]</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI
+CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI</t>
         </is>
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C002]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L403]</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C305]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [C002]</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -9231,9 +9239,10 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="F4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [C305]
+CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [C205]</t>
         </is>
       </c>
     </row>
@@ -9253,10 +9262,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L407]
-CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [L408]</t>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -9276,10 +9284,9 @@
           <t>14:30-15:30</t>
         </is>
       </c>
-      <c r="B6" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE [C102]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE [C203]</t>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -9314,27 +9321,27 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L406]
-CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L407]
+DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L405]</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L402]
-DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L404]</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C003]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L207]</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C002]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L207]</t>
+          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L208]
+CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [L107]</t>
         </is>
       </c>
     </row>
@@ -9354,21 +9361,22 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D8" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L407]
+DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L405]</t>
         </is>
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L402]
-DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L404]</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C003]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L207]</t>
         </is>
       </c>
       <c r="F8" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C002]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L207]</t>
+          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L208]
+CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [L107]</t>
         </is>
       </c>
     </row>
@@ -9428,7 +9436,7 @@
     <col width="60" customWidth="1" min="3" max="3"/>
     <col width="60" customWidth="1" min="4" max="4"/>
     <col width="60" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="60" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -9511,19 +9519,20 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr">
-        <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec B [C303]</t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec A [C303]
+MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [C001]</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec A [C303]</t>
         </is>
       </c>
     </row>
@@ -9545,7 +9554,8 @@
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | ECE [C004]</t>
+          <t>MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [C001]
+EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [L405]</t>
         </is>
       </c>
       <c r="E4" s="5" t="inlineStr">
@@ -9567,19 +9577,19 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C302]
-EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [C303]</t>
+          <t>EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C303]
+EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [C305]</t>
         </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec A [C303]
-MA262 (Multivariable Calculus) Sem 3 (Pre-Mid) | DSAI [L404]</t>
-        </is>
-      </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [C303]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec B [C303]
+MA262 (Multivariable Calculus) Sem 3 (Pre-Mid) | DSAI [L405]</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -9606,7 +9616,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | ECE [C004]</t>
+          <t>MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [C001]</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -9633,19 +9643,19 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Pre-Mid) | DSAI [L404]
-MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | DSAI [L404]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Pre-Mid) | DSAI [L405]
+MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | DSAI [L405]</t>
         </is>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | ECE [C004]
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | DSAI [L405]
 EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C205]</t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec A [C303]</t>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -9667,8 +9677,8 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C102]
-EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [C203]</t>
+          <t>EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C101]
+EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [C302]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -9747,7 +9757,7 @@
     <col width="60" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
     <col width="56" customWidth="1" min="4" max="4"/>
-    <col width="56" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -9794,10 +9804,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI [C204]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI [C205]</t>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
@@ -9829,8 +9838,8 @@
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C203]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [C204]</t>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C104]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C203]</t>
         </is>
       </c>
       <c r="D3" s="5" t="inlineStr">
@@ -9839,9 +9848,9 @@
 CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr">
-        <is>
-          <t>CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A</t>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -9858,14 +9867,13 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C203]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [C204]</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C101]
-CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A</t>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C104]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C203]</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -9893,12 +9901,12 @@
       <c r="B5" s="5" t="inlineStr">
         <is>
           <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [L207]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [L107]</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [L106]</t>
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -9926,13 +9934,13 @@
       <c r="B6" s="5" t="inlineStr">
         <is>
           <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [L207]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [L107]</t>
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [L208]</t>
         </is>
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [L106]
-CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A [L404]</t>
+          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A [L404]
+CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A [L405]</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -9957,14 +9965,15 @@
           <t>15:30-17:00</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C101]</t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A [C202]
+CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A [C302]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -9994,15 +10003,14 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t>CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A [C205]</t>
-        </is>
-      </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI
-CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI</t>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -10022,10 +10030,9 @@
           <t>18:30-20:00</t>
         </is>
       </c>
-      <c r="B9" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI [C204]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI [C205]</t>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
@@ -10033,10 +10040,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D9" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI [L107]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI [C204]</t>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -10072,8 +10078,8 @@
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="60" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
-    <col width="56" customWidth="1" min="4" max="4"/>
-    <col width="60" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -10120,10 +10126,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI [C204]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI [C205]</t>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
@@ -10150,14 +10155,14 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L408]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [C305]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L402]</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C203]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [C204]</t>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [C101]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [C202]</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -10165,9 +10170,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr">
-        <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [C303]</t>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -10184,14 +10189,14 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C203]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [C204]</t>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [C101]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [C202]</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C101]
-CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [C305]</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [C203]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [C302]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -10218,13 +10223,13 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [L207]
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [L106]
 CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [L107]</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [L106]</t>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -10232,9 +10237,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E5" s="5" t="inlineStr">
-        <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [C003]</t>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
@@ -10251,13 +10256,13 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [L207]
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [L106]
 CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [L107]</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [L106]</t>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -10265,9 +10270,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E6" s="5" t="inlineStr">
-        <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [C003]</t>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
@@ -10284,8 +10289,8 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C101]
-CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L107]</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L107]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L106]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -10317,7 +10322,8 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L107]</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L107]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L106]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -10325,10 +10331,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI
-CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI</t>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -10348,10 +10353,9 @@
           <t>18:30-20:00</t>
         </is>
       </c>
-      <c r="B9" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI [C204]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI [C205]</t>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
@@ -10359,10 +10363,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D9" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI [L107]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI [C204]</t>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -10810,7 +10813,7 @@
       </c>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec B [C305]</t>
+          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec B [C304]</t>
         </is>
       </c>
     </row>
@@ -10837,12 +10840,12 @@
       </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
-          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec A [C305]</t>
+          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec A [C304]</t>
         </is>
       </c>
       <c r="F4" s="5" t="inlineStr">
         <is>
-          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec A [C305]</t>
+          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec A [C304]</t>
         </is>
       </c>
     </row>
@@ -10869,7 +10872,7 @@
       </c>
       <c r="E5" s="5" t="inlineStr">
         <is>
-          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec B [C305]</t>
+          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec B [C304]</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
@@ -11027,8 +11030,8 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="60" customWidth="1" min="2" max="2"/>
-    <col width="60" customWidth="1" min="3" max="3"/>
-    <col width="60" customWidth="1" min="4" max="4"/>
+    <col width="56" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="60" customWidth="1" min="6" max="6"/>
   </cols>
@@ -11076,10 +11079,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI [C204]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI [C205]</t>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
@@ -11110,10 +11112,9 @@
 CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C203]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [C204]</t>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -11126,9 +11127,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="F3" s="5" t="inlineStr">
-        <is>
-          <t>CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [C104]</t>
+      <c r="F3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
     </row>
@@ -11138,15 +11139,15 @@
           <t>10:30-12:00</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C203]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [C204]</t>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C101]</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -11171,20 +11172,19 @@
           <t>13:00-14:30</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [L207]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [L107]</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [L106]</t>
-        </is>
-      </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L406]</t>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -11194,7 +11194,7 @@
       </c>
       <c r="F5" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L107]
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L208]
 CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [L207]</t>
         </is>
       </c>
@@ -11205,15 +11205,14 @@
           <t>14:30-15:30</t>
         </is>
       </c>
-      <c r="B6" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [L207]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [L107]</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [L106]</t>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -11228,7 +11227,7 @@
       </c>
       <c r="F6" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L107]
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L208]
 CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [L207]</t>
         </is>
       </c>
@@ -11239,9 +11238,9 @@
           <t>15:30-17:00</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C101]</t>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -11273,8 +11272,8 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [C303]
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [C001]</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [C304]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [C204]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -11282,10 +11281,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI
-CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI</t>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -11305,10 +11303,9 @@
           <t>18:30-20:00</t>
         </is>
       </c>
-      <c r="B9" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI [C204]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI [C205]</t>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
@@ -11316,10 +11313,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D9" s="5" t="inlineStr">
-        <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI [L107]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI [C204]</t>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -11353,11 +11349,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="56" customWidth="1" min="2" max="2"/>
-    <col width="56" customWidth="1" min="3" max="3"/>
-    <col width="57" customWidth="1" min="4" max="4"/>
-    <col width="57" customWidth="1" min="5" max="5"/>
-    <col width="57" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -11430,16 +11426,14 @@
           <t>09:00-10:30</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE
-CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE</t>
-        </is>
-      </c>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE
-CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE</t>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -11447,10 +11441,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C002]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L403]</t>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -11475,10 +11468,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [L403]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L404]</t>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -11508,10 +11500,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L407]
-CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [L408]</t>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -11531,10 +11522,9 @@
           <t>14:30-15:30</t>
         </is>
       </c>
-      <c r="B6" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE [C102]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE [C203]</t>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -11569,10 +11559,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L406]
-CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI</t>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -11585,10 +11574,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C002]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L207]</t>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
     </row>
@@ -11618,10 +11606,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="F8" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C002]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L207]</t>
+      <c r="F8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
     </row>
@@ -11756,14 +11743,14 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [C002]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [L403]</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [C305]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [C003]</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [C304]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [L402]</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -11891,7 +11878,7 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [L207]
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [L107]
 CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B</t>
         </is>
       </c>
@@ -11924,8 +11911,8 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [L207]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [C003]</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [L107]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [C004]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -12032,8 +12019,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="53" customWidth="1" min="2" max="2"/>
+    <col width="53" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
@@ -12146,9 +12133,10 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>HS152 (Economics/IET) Sem 1 (Pre-Mid) | ECE [C204]
+HS152 (Economics/IET) Sem 1 (Post-Mid) | ECE [C202]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -12237,9 +12225,10 @@
           <t>15:30-17:00</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>HS152 (Economics/IET) Sem 1 (Pre-Mid) | ECE [C204]
+HS152 (Economics/IET) Sem 1 (Post-Mid) | ECE [C205]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -13293,7 +13282,7 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="54" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
     <col width="54" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
@@ -13505,7 +13494,7 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>HS351 (Happiness &amp; Wellbeing) Sem 5 (Pre-Mid) | ECE
+          <t>HS351 (Happiness &amp; Wellbeing) Sem 5 (Pre-Mid) | ECE [L404]
 HS351 (Happiness &amp; Wellbeing) Sem 5 (Post-Mid) | ECE</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Added USER_MANUAL.md and modified README.md
</commit_message>
<xml_diff>
--- a/backend/output_timetables/Faculty_Availability_Schedule_Audit.xlsx
+++ b/backend/output_timetables/Faculty_Availability_Schedule_Audit.xlsx
@@ -624,7 +624,7 @@
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec B [C004]</t>
+          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec B [C003]</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -683,7 +683,7 @@
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec A [C004]</t>
+          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec A [C003]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -742,12 +742,12 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec A [C004]</t>
+          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec A [C003]</t>
         </is>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec B [C004]</t>
+          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec B [C003]</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -961,12 +961,12 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec B [C004]</t>
+          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec B [C003]</t>
         </is>
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec A [C004]</t>
+          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec A [C003]</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -998,8 +998,8 @@
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec B [C004]
-MA162 (Probability) Sem 1 (Pre-Mid) | ECE [C002]</t>
+          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec B [C003]
+MA162 (Probability) Sem 1 (Pre-Mid) | ECE [C004]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -1058,8 +1058,8 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec A [C004]
-MA162 (Probability) Sem 1 (Pre-Mid) | ECE [C002]</t>
+          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec A [C003]
+MA162 (Probability) Sem 1 (Pre-Mid) | ECE [C102]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -1339,8 +1339,8 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE [C302]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE [C101]</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE [C304]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE [C305]</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -1657,8 +1657,8 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [L402]
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [C205]</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [L407]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [L408]</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -1738,8 +1738,8 @@
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [C001]
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [C101]</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [C202]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [C203]</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -2013,8 +2013,8 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B [C203]
-CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec B [C305]</t>
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B [L402]
+CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec B [L405]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -2046,7 +2046,7 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B [C104]
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B [C101]
 CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec B [C204]</t>
         </is>
       </c>
@@ -2271,7 +2271,7 @@
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>DS161 (Introduction to DATA science and artificial intelligence) Sem 1 (Post-Mid) | ECE [C002]</t>
+          <t>DS161 (Introduction to DATA science and artificial intelligence) Sem 1 (Post-Mid) | ECE [C001]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -2330,7 +2330,7 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>DS161 (Introduction to DATA science and artificial intelligence) Sem 1 (Post-Mid) | ECE [C002]</t>
+          <t>DS161 (Introduction to DATA science and artificial intelligence) Sem 1 (Post-Mid) | ECE [C001]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -2679,8 +2679,8 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>EC351 (Introduction to Algorithms) Sem 5 (Pre-Mid) | ECE [L408]
-EC351 (Introduction to Algorithms) Sem 5 (Post-Mid) | ECE [C305]</t>
+          <t>EC351 (Introduction to Algorithms) Sem 5 (Pre-Mid) | ECE [L403]
+EC351 (Introduction to Algorithms) Sem 5 (Post-Mid) | ECE [L407]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -2928,8 +2928,8 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>EC301 (Introduction to VLSI Design) Sem 5 (Pre-Mid) | ECE [L404]
-EC301 (Introduction to VLSI Design) Sem 5 (Post-Mid) | ECE [L403]</t>
+          <t>EC301 (Introduction to VLSI Design) Sem 5 (Pre-Mid) | ECE
+EC301 (Introduction to VLSI Design) Sem 5 (Post-Mid) | ECE</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -3190,7 +3190,7 @@
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A [L408]
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A
 CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec A</t>
         </is>
       </c>
@@ -3315,8 +3315,8 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A [C203]
-CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec A [C202]</t>
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A [C205]
+CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec A [C102]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -3471,14 +3471,14 @@
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [C102]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [C305]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L406]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A</t>
         </is>
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [C004]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L403]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -3601,8 +3601,8 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L207]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L106]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L106]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L207]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -3634,8 +3634,8 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L207]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L106]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L106]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L207]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -4110,18 +4110,18 @@
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | DSAI [L407]
-MA261 (Differential Equations) Sem 3 (Post-Mid) | DSAI [L407]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | DSAI
+MA261 (Differential Equations) Sem 3 (Post-Mid) | DSAI [L403]</t>
         </is>
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec A [C001]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec A [L407]</t>
         </is>
       </c>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec A [C001]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec A [L407]</t>
         </is>
       </c>
     </row>
@@ -4148,7 +4148,7 @@
       </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec B [C001]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec B [L407]</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -4170,13 +4170,13 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec B [C001]
-MA261 (Differential Equations) Sem 3 (Post-Mid) | DSAI [L407]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec B [L407]
+MA261 (Differential Equations) Sem 3 (Post-Mid) | DSAI [L403]</t>
         </is>
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [C303]</t>
+          <t>MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [L406]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -4203,7 +4203,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [L407]</t>
+          <t>MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [C004]</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -4235,8 +4235,8 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | DSAI [C001]
-MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [L407]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | DSAI [L407]
+MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [C004]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -4423,8 +4423,8 @@
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [C302]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE [C303]</t>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [C104]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE [C204]</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -4451,8 +4451,8 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [C205]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE [C302]</t>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [C101]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE [C204]</t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
@@ -4784,7 +4784,7 @@
       </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
-          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [C302]</t>
+          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [C304]</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -4811,7 +4811,7 @@
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [L408]</t>
+          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [C303]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -4880,7 +4880,7 @@
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [L105]</t>
+          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
@@ -4912,7 +4912,7 @@
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [L105]</t>
+          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [C001]</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -5214,8 +5214,8 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec B [C305]
-CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec B [C002]</t>
+          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec B [C001]
+CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec B [C003]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -5380,14 +5380,14 @@
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [L402]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [L405]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B</t>
         </is>
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [C104]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [C302]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [C304]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [C305]</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -5441,8 +5441,8 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C204]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C205]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C302]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C303]</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -5479,13 +5479,13 @@
       </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C102]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C203]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C203]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C102]</t>
         </is>
       </c>
       <c r="E6" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [C102]
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [C203]
 CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [C101]</t>
         </is>
       </c>
@@ -5513,8 +5513,8 @@
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C104]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C202]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C204]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C302]</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -5706,8 +5706,8 @@
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [C004]
-EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [C102]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [C003]
+EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [C004]</t>
         </is>
       </c>
       <c r="F3" s="5" t="inlineStr">
@@ -5761,7 +5761,7 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [C004]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [C003]</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -5771,8 +5771,8 @@
       </c>
       <c r="E5" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [L105]
-EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [L206]
+EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [L105]</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
@@ -5804,8 +5804,8 @@
       </c>
       <c r="E6" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [L105]
-EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [C004]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [L206]
+EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [L105]</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
@@ -5822,7 +5822,7 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [C004]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [C003]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -5832,7 +5832,7 @@
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [C004]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [C003]</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
@@ -6046,8 +6046,8 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [C205]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [C305]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [C305]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [L403]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -6138,8 +6138,8 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [L402]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [L403]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [L404]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [L405]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -6149,7 +6149,7 @@
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [L207]
 CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B</t>
         </is>
       </c>
@@ -6182,8 +6182,8 @@
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [C002]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [C001]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [L207]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [L208]</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -6786,7 +6786,7 @@
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE [C002]</t>
+          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
@@ -6818,7 +6818,7 @@
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE [C002]</t>
+          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE [C101]</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -6995,13 +6995,13 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec A [C101]
+          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec A [C202]
 HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec A [C104]</t>
         </is>
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec B [C101]
+          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec B [C202]
 HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec B [C104]</t>
         </is>
       </c>
@@ -7029,8 +7029,8 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec B [C101]
-HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec B [C102]</t>
+          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec B [C202]
+HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec B [C104]</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -7089,8 +7089,8 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec A [C101]
-HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec A [C102]</t>
+          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec A [C202]
+HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec A [C104]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -7314,13 +7314,13 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec B [C004]</t>
+          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec B [C003]</t>
         </is>
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec A [C004]
-MA161 (Statistics) Sem 1 (Post-Mid) | ECE [C101]</t>
+          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec A [C003]
+MA161 (Statistics) Sem 1 (Post-Mid) | ECE [C001]</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -7347,8 +7347,8 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec A [C004]
-MA161 (Statistics) Sem 1 (Post-Mid) | ECE [C101]</t>
+          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec A [C003]
+MA161 (Statistics) Sem 1 (Post-Mid) | ECE [C001]</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -7358,7 +7358,7 @@
       </c>
       <c r="E5" s="5" t="inlineStr">
         <is>
-          <t>DA261 (Statistical Programming) Sem 3 (Post-Mid) | DSAI [L407]</t>
+          <t>DA261 (Statistical Programming) Sem 3 (Post-Mid) | DSAI [C101]</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
@@ -7407,7 +7407,7 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec B [C004]</t>
+          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec B [C003]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -7633,8 +7633,8 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [L403]
-CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [L404]</t>
+          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [L404]
+CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -7644,8 +7644,8 @@
       </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [L402]
-CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C205]</t>
+          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [C302]
+CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C204]</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -7758,13 +7758,13 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [C104]
-CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C205]</t>
+          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [C205]
+CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C202]</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>DS303 (Algorithms and Data Structures) Sem 5 (Pre-Mid) | DSAI [C303]
+          <t>DS303 (Algorithms and Data Structures) Sem 5 (Pre-Mid) | DSAI [C302]
 DS303 (Algorithms and Data Structures) Sem 5 (Post-Mid) | DSAI [C304]</t>
         </is>
       </c>
@@ -8708,8 +8708,8 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [C003]
-DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [C004]</t>
+          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [L405]
+DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [L406]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -8724,8 +8724,8 @@
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [C205]
-DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [C104]</t>
+          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [C302]
+DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [C303]</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -9105,8 +9105,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="54" customWidth="1" min="2" max="2"/>
-    <col width="54" customWidth="1" min="3" max="3"/>
+    <col width="47" customWidth="1" min="2" max="2"/>
+    <col width="47" customWidth="1" min="3" max="3"/>
     <col width="57" customWidth="1" min="4" max="4"/>
     <col width="57" customWidth="1" min="5" max="5"/>
     <col width="57" customWidth="1" min="6" max="6"/>
@@ -9184,14 +9184,14 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L406]
-DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L408]</t>
+          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI
+DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L404]
-DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L406]</t>
+          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI
+DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI</t>
         </is>
       </c>
       <c r="D3" s="5" t="inlineStr">
@@ -9202,8 +9202,8 @@
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C305]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [C002]</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C001]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L402]</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -9230,8 +9230,8 @@
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [L403]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L404]</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C305]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L402]</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -9241,8 +9241,8 @@
       </c>
       <c r="F4" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [C305]
-CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [C205]</t>
+          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [C204]
+CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [C304]</t>
         </is>
       </c>
     </row>
@@ -9328,20 +9328,20 @@
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L407]
+          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L406]
 DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L405]</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C003]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L207]</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C004]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L106]</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L208]
-CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [L107]</t>
+          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L207]
+CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [L106]</t>
         </is>
       </c>
     </row>
@@ -9363,20 +9363,20 @@
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
-          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L407]
+          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L406]
 DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L405]</t>
         </is>
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C003]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L207]</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C004]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L106]</t>
         </is>
       </c>
       <c r="F8" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L208]
-CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [L107]</t>
+          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L207]
+CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [L106]</t>
         </is>
       </c>
     </row>
@@ -9526,13 +9526,13 @@
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec A [C303]
-MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [C001]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec A [L406]
+MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [C303]</t>
         </is>
       </c>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec A [C303]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec A [L406]</t>
         </is>
       </c>
     </row>
@@ -9554,13 +9554,13 @@
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [C001]
+          <t>MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [L407]
 EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [L405]</t>
         </is>
       </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec B [C303]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec B [L406]</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -9577,14 +9577,14 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C303]
+          <t>EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C304]
 EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [C305]</t>
         </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec B [C303]
-MA262 (Multivariable Calculus) Sem 3 (Pre-Mid) | DSAI [L405]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec B [L406]
+MA262 (Multivariable Calculus) Sem 3 (Pre-Mid) | DSAI [L408]</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -9616,7 +9616,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [C001]</t>
+          <t>MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [C303]</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -9643,14 +9643,14 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Pre-Mid) | DSAI [L405]
-MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | DSAI [L405]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Pre-Mid) | DSAI [L408]
+MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | DSAI [L408]</t>
         </is>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | DSAI [L405]
-EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C205]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | DSAI [L408]
+EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C303]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -9678,7 +9678,7 @@
       <c r="B8" s="5" t="inlineStr">
         <is>
           <t>EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C101]
-EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [C302]</t>
+EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [C102]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -9839,7 +9839,7 @@
       <c r="C3" s="5" t="inlineStr">
         <is>
           <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C104]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C203]</t>
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C205]</t>
         </is>
       </c>
       <c r="D3" s="5" t="inlineStr">
@@ -9868,7 +9868,7 @@
       <c r="B4" s="5" t="inlineStr">
         <is>
           <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C104]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C203]</t>
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C205]</t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
@@ -9900,7 +9900,7 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [L207]
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B
 CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B</t>
         </is>
       </c>
@@ -9933,14 +9933,14 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [L207]
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [L106]
 CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [L208]</t>
         </is>
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A [L404]
-CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A [L405]</t>
+          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A [L406]
+CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A [L407]</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -9972,8 +9972,8 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A [C202]
-CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A [C302]</t>
+          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A [C304]
+CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A [L403]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -10155,8 +10155,8 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [C305]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L402]</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L408]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
@@ -10195,8 +10195,8 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [C203]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [C302]</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [C204]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L402]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -10223,8 +10223,8 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [L106]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [L107]</t>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [L207]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -10256,7 +10256,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [L106]
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [L207]
 CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [L107]</t>
         </is>
       </c>
@@ -10290,7 +10290,7 @@
       <c r="B7" s="5" t="inlineStr">
         <is>
           <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L107]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L106]</t>
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L207]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -10323,7 +10323,7 @@
       <c r="B8" s="5" t="inlineStr">
         <is>
           <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L107]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L106]</t>
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L207]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -10813,7 +10813,7 @@
       </c>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec B [C304]</t>
+          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec B [C305]</t>
         </is>
       </c>
     </row>
@@ -10840,12 +10840,12 @@
       </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
-          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec A [C304]</t>
+          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec A [C305]</t>
         </is>
       </c>
       <c r="F4" s="5" t="inlineStr">
         <is>
-          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec A [C304]</t>
+          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec A [C305]</t>
         </is>
       </c>
     </row>
@@ -10872,7 +10872,7 @@
       </c>
       <c r="E5" s="5" t="inlineStr">
         <is>
-          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec B [C304]</t>
+          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec B [C305]</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
@@ -11194,8 +11194,8 @@
       </c>
       <c r="F5" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L208]
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [L207]</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L107]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [L106]</t>
         </is>
       </c>
     </row>
@@ -11227,8 +11227,8 @@
       </c>
       <c r="F6" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L208]
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [L207]</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L107]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [L106]</t>
         </is>
       </c>
     </row>
@@ -11272,8 +11272,8 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [C304]
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [C204]</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [C305]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [C002]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -11743,14 +11743,14 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [C002]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [L403]</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [C304]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [L402]</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -11912,7 +11912,7 @@
       <c r="C8" s="5" t="inlineStr">
         <is>
           <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [L107]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [C004]</t>
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [L208]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -12135,8 +12135,8 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>HS152 (Economics/IET) Sem 1 (Pre-Mid) | ECE [C204]
-HS152 (Economics/IET) Sem 1 (Post-Mid) | ECE [C202]</t>
+          <t>HS152 (Economics/IET) Sem 1 (Pre-Mid) | ECE [C104]
+HS152 (Economics/IET) Sem 1 (Post-Mid) | ECE [C102]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -12227,8 +12227,8 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>HS152 (Economics/IET) Sem 1 (Pre-Mid) | ECE [C204]
-HS152 (Economics/IET) Sem 1 (Post-Mid) | ECE [C205]</t>
+          <t>HS152 (Economics/IET) Sem 1 (Pre-Mid) | ECE [C104]
+HS152 (Economics/IET) Sem 1 (Post-Mid) | ECE [C202]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -13282,7 +13282,7 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="60" customWidth="1" min="3" max="3"/>
+    <col width="54" customWidth="1" min="3" max="3"/>
     <col width="54" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
@@ -13494,7 +13494,7 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>HS351 (Happiness &amp; Wellbeing) Sem 5 (Pre-Mid) | ECE [L404]
+          <t>HS351 (Happiness &amp; Wellbeing) Sem 5 (Pre-Mid) | ECE
 HS351 (Happiness &amp; Wellbeing) Sem 5 (Post-Mid) | ECE</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Improved classroom scheduling logic
</commit_message>
<xml_diff>
--- a/backend/output_timetables/Faculty_Availability_Schedule_Audit.xlsx
+++ b/backend/output_timetables/Faculty_Availability_Schedule_Audit.xlsx
@@ -49,6 +49,7 @@
     <sheet name="Utkarsh K" sheetId="40" state="visible" r:id="rId40"/>
     <sheet name="Vivekraj" sheetId="41" state="visible" r:id="rId41"/>
     <sheet name="CONFLICT_SUMMARY" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="CONFLICT_CATEGORIES" sheetId="43" state="visible" r:id="rId43"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -139,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -154,6 +155,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -533,7 +537,7 @@
     <col width="18" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
     <col width="60" customWidth="1" min="4" max="4"/>
-    <col width="60" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -622,9 +626,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr">
-        <is>
-          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec B [C003]</t>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -683,7 +687,7 @@
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec A [C003]</t>
+          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec B [C305]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -742,12 +746,12 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec A [C003]</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec B [C003]</t>
+          <t>DS161 (Introduction to data science and artifical inteligance) Sem 1 (Pre-Mid) | CSE Sec B [C305]</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -845,7 +849,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="48" customWidth="1" min="2" max="2"/>
+    <col width="57" customWidth="1" min="2" max="2"/>
     <col width="57" customWidth="1" min="3" max="3"/>
     <col width="57" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
@@ -934,7 +938,7 @@
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>MA263 (Random Processes) Sem 3 (Pre-Mid) | ECE</t>
+          <t>MA263 (Random Processes) Sem 3 (Pre-Mid) | ECE [L207]</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -956,17 +960,19 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>MA263 (Random Processes) Sem 3 (Pre-Mid) | ECE</t>
+          <t>MA263 (Random Processes) Sem 3 (Pre-Mid) | ECE [L208]</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec B [C003]</t>
+          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec B [C202]
+MA162 (Probability) Sem 1 (Pre-Mid) | DSAI [C304]</t>
         </is>
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec A [C003]</t>
+          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec A [C202]
+MA162 (Probability) Sem 1 (Pre-Mid) | DSAI [C304]</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -991,15 +997,14 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec A [C202]</t>
         </is>
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec B [C003]
-MA162 (Probability) Sem 1 (Pre-Mid) | ECE [C004]</t>
+          <t>MA162 (Probability) Sem 1 (Pre-Mid) | ECE [C304]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -1051,15 +1056,14 @@
           <t>15:30-17:00</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec B [C202]</t>
         </is>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>MA162 (Probability) Sem 1 (Post-Mid) | CSE Sec A [C003]
-MA162 (Probability) Sem 1 (Pre-Mid) | ECE [C102]</t>
+          <t>MA162 (Probability) Sem 1 (Pre-Mid) | ECE [C304]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -1163,7 +1167,7 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="56" customWidth="1" min="2" max="2"/>
-    <col width="49" customWidth="1" min="3" max="3"/>
+    <col width="56" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
@@ -1241,14 +1245,14 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE
-CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE [L407]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE [L406]</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE
-CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE [L107]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE [L207]</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -1339,8 +1343,8 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE [C304]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE [C305]</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | ECE [C305]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | ECE [C302]</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -1481,7 +1485,7 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="60" customWidth="1" min="2" max="2"/>
-    <col width="56" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="60" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
@@ -1559,14 +1563,14 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [L404]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [L404]</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [L404]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [L404]</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -1657,8 +1661,8 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [L407]
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [L408]</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [C204]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [C303]</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -1705,8 +1709,8 @@
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [L107]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [C307]</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
@@ -1738,8 +1742,8 @@
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [C202]
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [C203]</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec B [L107]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec B [C307]</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -1921,8 +1925,8 @@
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B
-CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec B</t>
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B [L106]
+CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec B [L105]</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -2013,8 +2017,8 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B [L402]
-CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec B [L405]</t>
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B [L405]
+CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec B [L408]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -2046,8 +2050,8 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B [C101]
-CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec B [C204]</t>
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec B [C002]
+CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec B [C302]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -2237,9 +2241,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>DS161 (Introduction to DS and AI) Sem 1 (Post-Mid) | DSAI [C302]</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -2264,14 +2268,14 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>DS161 (Introduction to DS and AI) Sem 1 (Post-Mid) | DSAI [C302]</t>
         </is>
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>DS161 (Introduction to DATA science and artificial intelligence) Sem 1 (Post-Mid) | ECE [C001]</t>
+          <t>DS161 (Introduction to DATA science and artificial intelligence) Sem 1 (Post-Mid) | ECE [C101]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -2330,7 +2334,7 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>DS161 (Introduction to DATA science and artificial intelligence) Sem 1 (Post-Mid) | ECE [C001]</t>
+          <t>DS161 (Introduction to DATA science and artificial intelligence) Sem 1 (Post-Mid) | ECE [C101]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -2435,7 +2439,7 @@
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
-    <col width="59" customWidth="1" min="4" max="4"/>
+    <col width="60" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
@@ -2554,8 +2558,8 @@
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>EC351 (Introduction to Algorithms) Sem 5 (Pre-Mid) | ECE
-EC351 (Introduction to Algorithms) Sem 5 (Post-Mid) | ECE</t>
+          <t>EC351 (Introduction to Algorithms) Sem 5 (Pre-Mid) | ECE [L404]
+EC351 (Introduction to Algorithms) Sem 5 (Post-Mid) | ECE [L404]</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -2582,8 +2586,8 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>EC351 (Introduction to Algorithms) Sem 5 (Pre-Mid) | ECE
-EC351 (Introduction to Algorithms) Sem 5 (Post-Mid) | ECE</t>
+          <t>EC351 (Introduction to Algorithms) Sem 5 (Pre-Mid) | ECE [L106]
+EC351 (Introduction to Algorithms) Sem 5 (Post-Mid) | ECE [C308]</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -2679,8 +2683,8 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>EC351 (Introduction to Algorithms) Sem 5 (Pre-Mid) | ECE [L403]
-EC351 (Introduction to Algorithms) Sem 5 (Post-Mid) | ECE [L407]</t>
+          <t>EC351 (Introduction to Algorithms) Sem 5 (Pre-Mid) | ECE [L406]
+EC351 (Introduction to Algorithms) Sem 5 (Post-Mid) | ECE [C202]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -2830,14 +2834,14 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>EC301 (Introduction to VLSI Design) Sem 5 (Pre-Mid) | ECE
-EC301 (Introduction to VLSI Design) Sem 5 (Post-Mid) | ECE</t>
+          <t>EC301 (Introduction to VLSI Design) Sem 5 (Pre-Mid) | ECE [L404]
+EC301 (Introduction to VLSI Design) Sem 5 (Post-Mid) | ECE [L404]</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>EC301 (Introduction to VLSI Design) Sem 5 (Pre-Mid) | ECE
-EC301 (Introduction to VLSI Design) Sem 5 (Post-Mid) | ECE</t>
+          <t>EC301 (Introduction to VLSI Design) Sem 5 (Pre-Mid) | ECE [L404]
+EC301 (Introduction to VLSI Design) Sem 5 (Post-Mid) | ECE [L404]</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -2928,8 +2932,8 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>EC301 (Introduction to VLSI Design) Sem 5 (Pre-Mid) | ECE
-EC301 (Introduction to VLSI Design) Sem 5 (Post-Mid) | ECE</t>
+          <t>EC301 (Introduction to VLSI Design) Sem 5 (Pre-Mid) | ECE [C003]
+EC301 (Introduction to VLSI Design) Sem 5 (Post-Mid) | ECE [L405]</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -3071,7 +3075,7 @@
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="60" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
-    <col width="60" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
@@ -3151,9 +3155,10 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A [L404]
+CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec A [L404]</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -3188,10 +3193,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A
-CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec A</t>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -3213,8 +3217,8 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A
-CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec A</t>
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A [C003]
+CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec A [L404]</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -3244,9 +3248,10 @@
           <t>14:30-15:30</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A [C002]
+CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec A [C304]</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -3313,10 +3318,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t>CS304 (Artificial Intelligence) Sem 5 (Pre-Mid) | CSE Sec A [C205]
-CS304 (Artificial Intelligence) Sem 5 (Post-Mid) | CSE Sec A [C102]</t>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -3469,16 +3473,15 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L406]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A</t>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [C308]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L106]</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -3503,9 +3506,10 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [C303]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [C305]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -3601,8 +3605,8 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L106]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L207]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L105]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L107]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -3634,8 +3638,8 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L106]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L207]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec A [L105]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec A [L107]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -4110,18 +4114,18 @@
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | DSAI
-MA261 (Differential Equations) Sem 3 (Post-Mid) | DSAI [L403]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | DSAI [L105]
+MA261 (Differential Equations) Sem 3 (Post-Mid) | DSAI [C101]</t>
         </is>
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec A [L407]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec A [C307]</t>
         </is>
       </c>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec A [L407]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec A [C307]</t>
         </is>
       </c>
     </row>
@@ -4148,7 +4152,7 @@
       </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec B [L407]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec B [C307]</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -4170,13 +4174,13 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec B [L407]
-MA261 (Differential Equations) Sem 3 (Post-Mid) | DSAI [L403]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | CSE Sec B [C307]
+MA261 (Differential Equations) Sem 3 (Post-Mid) | DSAI [C101]</t>
         </is>
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [L406]</t>
+          <t>MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [L404]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -4203,7 +4207,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [C004]</t>
+          <t>MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [L407]</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -4235,8 +4239,8 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | DSAI [L407]
-MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [C004]</t>
+          <t>MA261 (Differential Equations) Sem 3 (Pre-Mid) | DSAI [C307]
+MA262 (Differential Equations) Sem 3 (Post-Mid) | ECE [L407]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -4423,8 +4427,8 @@
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [C104]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE [C204]</t>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [C101]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE [C203]</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -4451,8 +4455,8 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [C101]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE [C204]</t>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [C204]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE [C002]</t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
@@ -4484,8 +4488,8 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE
-CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE</t>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [L107]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE [L208]</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -4517,7 +4521,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [L208]
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | ECE [L107]
 CS161 (Problem Solving) Sem 1 (Post-Mid) | ECE [L208]</t>
         </is>
       </c>
@@ -4784,7 +4788,7 @@
       </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
-          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [C304]</t>
+          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [L106]</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -4811,7 +4815,7 @@
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [C303]</t>
+          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [C003]</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -4880,7 +4884,7 @@
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE</t>
+          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [L206]</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
@@ -4912,7 +4916,7 @@
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [C001]</t>
+          <t>EC262 (Semiconductor Devices) Sem 3 (Pre-Mid) | ECE [L206]</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -4974,7 +4978,7 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="60" customWidth="1" min="2" max="2"/>
-    <col width="56" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
@@ -5084,14 +5088,14 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec B
-CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec B</t>
+          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec B [L404]
+CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec B [L404]</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec B
-CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec B</t>
+          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec B [L407]
+CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec B [L406]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -5214,8 +5218,8 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec B [C001]
-CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec B [C003]</t>
+          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec B [C304]
+CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec B [C305]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -5380,14 +5384,14 @@
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [L208]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [C307]</t>
         </is>
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [C304]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [C305]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [C102]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [C303]</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -5441,8 +5445,8 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C302]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C303]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C104]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C204]</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -5479,14 +5483,14 @@
       </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C203]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C102]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C104]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C203]</t>
         </is>
       </c>
       <c r="E6" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [C203]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [C101]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec B [C305]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec B [C002]</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
@@ -5513,8 +5517,8 @@
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C204]
-CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C302]</t>
+          <t>CS264 (Computer Networks) Sem 3 (Pre-Mid) | CSE Sec A [C102]
+CS264 (Computer Networks) Sem 3 (Post-Mid) | CSE Sec A [C303]</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -5612,11 +5616,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="60" customWidth="1" min="2" max="2"/>
+    <col width="54" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
     <col width="60" customWidth="1" min="4" max="4"/>
     <col width="60" customWidth="1" min="5" max="5"/>
-    <col width="53" customWidth="1" min="6" max="6"/>
+    <col width="60" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5706,13 +5710,14 @@
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [C003]
-EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [C004]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [C304]
+EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [C202]</t>
         </is>
       </c>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [C004]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [C304]
+EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [C205]</t>
         </is>
       </c>
     </row>
@@ -5761,18 +5766,18 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [C003]</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+          <t>EC161 (Digital Design) Sem 1 (Pre-Mid) | DSAI [C202]</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [C304]</t>
         </is>
       </c>
       <c r="E5" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [L206]
-EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [L105]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [L105]
+EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [L206]</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
@@ -5804,8 +5809,8 @@
       </c>
       <c r="E6" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [L206]
-EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [L105]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [L105]
+EC161 (Digital Design) Sem 1 (Pre-Mid) | ECE [L206]</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
@@ -5822,22 +5827,23 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [C003]</t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+          <t>EC161 (Digital Design) Sem 1 (Pre-Mid) | DSAI [C202]</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [C304]</t>
         </is>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [C003]</t>
-        </is>
-      </c>
-      <c r="E7" s="5" t="inlineStr">
-        <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [L206]</t>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [L105]
+EC161 (Digital Design) Sem 1 (Pre-Mid) | DSAI [L206]</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
@@ -5862,14 +5868,15 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D8" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
-        </is>
-      </c>
-      <c r="E8" s="5" t="inlineStr">
-        <is>
-          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec B [L206]</t>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>EC161 (Digital Design) Sem 1 (Post-Mid) | CSE Sec A [L105]
+EC161 (Digital Design) Sem 1 (Pre-Mid) | DSAI [L206]</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -6046,8 +6053,8 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [C305]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [L403]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [C203]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [C002]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -6138,8 +6145,8 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [L404]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [L405]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [C002]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [C001]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -6149,8 +6156,8 @@
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [L207]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [L105]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [L106]</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -6182,8 +6189,8 @@
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
-          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [L207]
-CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [L208]</t>
+          <t>CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Pre-Mid) | CSE Sec B [L105]
+CS263 (Design &amp; Analysis of Algorithms) Sem 3 (Post-Mid) | CSE Sec B [L106]</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -6564,8 +6571,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="51" customWidth="1" min="2" max="2"/>
-    <col width="51" customWidth="1" min="3" max="3"/>
+    <col width="58" customWidth="1" min="2" max="2"/>
+    <col width="58" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="58" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
@@ -6675,12 +6682,12 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE</t>
+          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE [L107]</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE</t>
+          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE [C004]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -6786,7 +6793,7 @@
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE</t>
+          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE [L105]</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
@@ -6818,7 +6825,7 @@
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE [C101]</t>
+          <t>EC263 (Analog Electronics) Sem 3 (Post-Mid) | ECE [L105]</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -6995,14 +7002,13 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec A [C202]
-HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec A [C104]</t>
+          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec B [C205]
+HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec A [C204]</t>
         </is>
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec B [C202]
-HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec B [C104]</t>
+          <t>HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec B [C205]</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -7029,8 +7035,7 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec B [C202]
-HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec B [C104]</t>
+          <t>HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec B [C205]</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -7089,8 +7094,8 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec A [C202]
-HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec A [C104]</t>
+          <t>HS161 (English Language) Sem 1 (Pre-Mid) | CSE Sec B [C205]
+HS161 (English Language) Sem 1 (Post-Mid) | CSE Sec A [C303]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -7198,11 +7203,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="55" customWidth="1" min="2" max="2"/>
+    <col width="51" customWidth="1" min="2" max="2"/>
     <col width="55" customWidth="1" min="3" max="3"/>
     <col width="55" customWidth="1" min="4" max="4"/>
     <col width="60" customWidth="1" min="5" max="5"/>
-    <col width="60" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7314,18 +7319,18 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec B [C003]</t>
+          <t>MA161 (Statistics) Sem 1 (Post-Mid) | DSAI [C102]</t>
         </is>
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec A [C003]
-MA161 (Statistics) Sem 1 (Post-Mid) | ECE [C001]</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec B [C302]
+MA161 (Statistics) Sem 1 (Post-Mid) | ECE [C102]</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>DA261 (Statistical Programming) Sem 3 (Post-Mid) | DSAI [C102]</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -7347,8 +7352,8 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec A [C003]
-MA161 (Statistics) Sem 1 (Post-Mid) | ECE [C001]</t>
+          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec B [C302]
+MA161 (Statistics) Sem 1 (Post-Mid) | ECE [C102]</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -7358,7 +7363,7 @@
       </c>
       <c r="E5" s="5" t="inlineStr">
         <is>
-          <t>DA261 (Statistical Programming) Sem 3 (Post-Mid) | DSAI [C101]</t>
+          <t>DA261 (Statistical Programming) Sem 3 (Post-Mid) | DSAI</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
@@ -7388,9 +7393,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E6" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>DA261 (Statistical Programming) Sem 3 (Post-Mid) | DSAI [C001]</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
@@ -7407,7 +7412,7 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>MA161 (Statistics) Sem 1 (Pre-Mid) | CSE Sec B [C003]</t>
+          <t>MA161 (Statistics) Sem 1 (Post-Mid) | DSAI [C102]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -7425,9 +7430,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>DA261 (Statistical Programming) Sem 3 (Post-Mid) | DSAI [L403]</t>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
     </row>
@@ -7457,9 +7462,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="F8" s="5" t="inlineStr">
-        <is>
-          <t>DA261 (Statistical Programming) Sem 3 (Post-Mid) | DSAI [L403]</t>
+      <c r="F8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
     </row>
@@ -7517,8 +7522,8 @@
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="60" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="60" customWidth="1" min="5" max="5"/>
+    <col width="60" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -7594,14 +7599,14 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>DS303 (Algorithms and Data Structures) Sem 5 (Pre-Mid) | DSAI
-DS303 (Algorithms and Data Structures) Sem 5 (Post-Mid) | DSAI</t>
+          <t>DS303 (Algorithms and Data Structures) Sem 5 (Pre-Mid) | DSAI [L404]
+DS303 (Algorithms and Data Structures) Sem 5 (Post-Mid) | DSAI [L404]</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>DS303 (Algorithms and Data Structures) Sem 5 (Pre-Mid) | DSAI
-DS303 (Algorithms and Data Structures) Sem 5 (Post-Mid) | DSAI</t>
+          <t>DS303 (Algorithms and Data Structures) Sem 5 (Pre-Mid) | DSAI [L404]
+DS303 (Algorithms and Data Structures) Sem 5 (Post-Mid) | DSAI [L404]</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -7633,19 +7638,19 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [L404]
-CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
-        </is>
-      </c>
-      <c r="E4" s="5" t="inlineStr">
-        <is>
-          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [C302]
-CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C204]</t>
+          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [L206]
+CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C003]</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [L206]
+CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [L408]</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -7758,14 +7763,14 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [C205]
-CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C202]</t>
+          <t>CS304 (Artificial Intelligence) Sem 3 (Pre-Mid) | DSAI [C102]
+CS304 (Artificial Intelligence) Sem 3 (Post-Mid) | DSAI [C303]</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>DS303 (Algorithms and Data Structures) Sem 5 (Pre-Mid) | DSAI [C302]
-DS303 (Algorithms and Data Structures) Sem 5 (Post-Mid) | DSAI [C304]</t>
+          <t>DS303 (Algorithms and Data Structures) Sem 5 (Pre-Mid) | DSAI [L405]
+DS303 (Algorithms and Data Structures) Sem 5 (Post-Mid) | DSAI [C102]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -8467,7 +8472,7 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="60" customWidth="1" min="2" max="2"/>
-    <col width="56" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="60" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
@@ -8577,14 +8582,14 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI
-DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI</t>
+          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [L404]
+DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [L404]</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI
-DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI</t>
+          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [L208]
+DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [L105]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -8690,7 +8695,7 @@
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI
+          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [C308]
 DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI</t>
         </is>
       </c>
@@ -8708,8 +8713,8 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [L405]
-DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [L406]</t>
+          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [C001]
+DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [C002]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -8724,8 +8729,8 @@
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [C302]
-DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [C303]</t>
+          <t>DS302 (Computer Communication) Sem 5 (Pre-Mid) | DSAI [C308]
+DS302 (Computer Communication) Sem 5 (Post-Mid) | DSAI [C004]</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -8787,7 +8792,7 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="60" customWidth="1" min="2" max="2"/>
-    <col width="58" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
@@ -8897,14 +8902,14 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>EC306 (Digital Signal Processing) Sem 5 (Pre-Mid) | ECE
-EC306 (Digital Signal Processing) Sem 5 (Post-Mid) | ECE</t>
+          <t>EC306 (Digital Signal Processing) Sem 5 (Pre-Mid) | ECE [L404]
+EC306 (Digital Signal Processing) Sem 5 (Post-Mid) | ECE [L404]</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>EC306 (Digital Signal Processing) Sem 5 (Pre-Mid) | ECE
-EC306 (Digital Signal Processing) Sem 5 (Post-Mid) | ECE</t>
+          <t>EC306 (Digital Signal Processing) Sem 5 (Pre-Mid) | ECE [L107]
+EC306 (Digital Signal Processing) Sem 5 (Post-Mid) | ECE [L404]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -9105,8 +9110,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="47" customWidth="1" min="2" max="2"/>
-    <col width="47" customWidth="1" min="3" max="3"/>
+    <col width="54" customWidth="1" min="2" max="2"/>
+    <col width="57" customWidth="1" min="3" max="3"/>
     <col width="57" customWidth="1" min="4" max="4"/>
     <col width="57" customWidth="1" min="5" max="5"/>
     <col width="57" customWidth="1" min="6" max="6"/>
@@ -9184,31 +9189,32 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI
-DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI</t>
+          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L207]
+DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L405]</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI
-DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI</t>
+          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L208]
+DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L106]</t>
         </is>
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI
-CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI</t>
+          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L404]
+CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [L404]</t>
         </is>
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C001]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L402]</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [L406]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [C204]</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [L406]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [C102]</t>
         </is>
       </c>
     </row>
@@ -9228,10 +9234,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C305]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L402]</t>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -9239,10 +9244,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="F4" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [C204]
-CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [C304]</t>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
     </row>
@@ -9321,27 +9325,27 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L402]
+CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [L403]</t>
         </is>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L406]
-DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L405]</t>
-        </is>
-      </c>
-      <c r="E7" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C004]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L106]</t>
+          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [C308]
+DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L207]
-CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [L106]</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [L207]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L107]</t>
         </is>
       </c>
     </row>
@@ -9363,20 +9367,19 @@
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
-          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [L406]
-DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [L405]</t>
-        </is>
-      </c>
-      <c r="E8" s="5" t="inlineStr">
-        <is>
-          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [C004]
-CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L106]</t>
+          <t>DA262 (Data Handling) Sem 3 (Pre-Mid) | DSAI [C308]
+DA262 (Data Handling) Sem 3 (Post-Mid) | DSAI [C104]</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="F8" s="5" t="inlineStr">
         <is>
-          <t>CS307 (Machine Learning) Sem 5 (Pre-Mid) | DSAI [L207]
-CS307 (Machine Learning) Sem 5 (Post-Mid) | DSAI [L106]</t>
+          <t>CS307 (Machine Learning) Sem 3 (Pre-Mid) | DSAI [L207]
+CS307 (Machine Learning) Sem 3 (Post-Mid) | DSAI [L107]</t>
         </is>
       </c>
     </row>
@@ -9526,13 +9529,13 @@
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec A [L406]
-MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [C303]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec A [L404]
+MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [C104]</t>
         </is>
       </c>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec A [L406]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec A [L404]</t>
         </is>
       </c>
     </row>
@@ -9554,13 +9557,13 @@
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [L407]
-EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [L405]</t>
+          <t>MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [C307]
+EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [L403]</t>
         </is>
       </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec B [L406]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec B [L404]</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -9578,13 +9581,13 @@
       <c r="B5" s="5" t="inlineStr">
         <is>
           <t>EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C304]
-EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [C305]</t>
+EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [C001]</t>
         </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec B [L406]
-MA262 (Multivariable Calculus) Sem 3 (Pre-Mid) | DSAI [L408]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | CSE Sec B [L404]
+MA262 (Multivariable Calculus) Sem 3 (Pre-Mid) | DSAI [L403]</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -9616,7 +9619,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [C303]</t>
+          <t>MA261 (Multivariable Calculus) Sem 3 (Pre-Mid) | ECE [C104]</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -9643,14 +9646,14 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Pre-Mid) | DSAI [L408]
-MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | DSAI [L408]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Pre-Mid) | DSAI [L404]
+MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | DSAI [L403]</t>
         </is>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | DSAI [L408]
-EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C303]</t>
+          <t>MA262 (Multivariable Calculus) Sem 3 (Post-Mid) | DSAI [L403]
+EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [L407]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -9677,8 +9680,8 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C101]
-EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [C102]</t>
+          <t>EC261 (Signals &amp; Systems) Sem 3 (Pre-Mid) | ECE [C302]
+EC261 (Signals &amp; Systems) Sem 3 (Post-Mid) | ECE [C204]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -9756,7 +9759,7 @@
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="60" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
-    <col width="56" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
@@ -9838,14 +9841,13 @@
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C104]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C205]</t>
-        </is>
-      </c>
-      <c r="D3" s="5" t="inlineStr">
-        <is>
-          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A
-CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A</t>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C304]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C204]</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -9867,13 +9869,17 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C104]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C205]</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+          <t>⚠ DOUBLE-BOOKING:
+CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [C304]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C302]
+CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A [L206]
+CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A [L404]</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A [L403]
+CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A [L402]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -9900,7 +9906,7 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [L207]
 CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B</t>
         </is>
       </c>
@@ -9933,14 +9939,13 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [L106]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [L208]</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A [L406]
-CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A [L407]</t>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec B [L207]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec B [C004]</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -9970,10 +9975,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A [C304]
-CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A [L403]</t>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -9998,9 +10002,10 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>CS309 (Statistics for CS) Sem 5 (Pre-Mid) | CSE Sec A [C205]
+CS309 (Statistics for CS) Sem 5 (Post-Mid) | CSE Sec A [C203]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -10155,14 +10160,17 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L408]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L208]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L107]</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [C101]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [C202]</t>
+          <t>⚠ DOUBLE-BOOKING:
+CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [C101]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [C104]
+CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L405]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L406]</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -10190,13 +10198,12 @@
       <c r="B4" s="5" t="inlineStr">
         <is>
           <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [C101]
-CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [C202]</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [C204]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L402]</t>
+CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [C203]</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -10223,7 +10230,7 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [L207]
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [L106]
 CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A</t>
         </is>
       </c>
@@ -10256,7 +10263,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [L207]
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | CSE Sec A [L106]
 CS161 (Problem Solving) Sem 1 (Post-Mid) | CSE Sec A [L107]</t>
         </is>
       </c>
@@ -10289,8 +10296,8 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L107]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L207]</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L207]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L107]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -10322,8 +10329,8 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L107]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L207]</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec A [L207]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec A [L107]</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -10813,7 +10820,7 @@
       </c>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec B [C305]</t>
+          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec B [C303]</t>
         </is>
       </c>
     </row>
@@ -10840,12 +10847,12 @@
       </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
-          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec A [C305]</t>
+          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec A [C303]</t>
         </is>
       </c>
       <c r="F4" s="5" t="inlineStr">
         <is>
-          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec A [C305]</t>
+          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec A [C303]</t>
         </is>
       </c>
     </row>
@@ -10872,7 +10879,7 @@
       </c>
       <c r="E5" s="5" t="inlineStr">
         <is>
-          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec B [C305]</t>
+          <t>CS261 (Operating systems) Sem 3 (Pre-Mid) | CSE Sec B [C302]</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
@@ -11030,10 +11037,10 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="60" customWidth="1" min="2" max="2"/>
-    <col width="56" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="60" customWidth="1" min="6" max="6"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="4" max="4"/>
+    <col width="60" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -11108,13 +11115,14 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L404]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [L404]</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI [C303]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI [C302]</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -11139,20 +11147,21 @@
           <t>10:30-12:00</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI [C101]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI [C104]</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [C308]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [L208]</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -11172,9 +11181,10 @@
           <t>13:00-14:30</t>
         </is>
       </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI [L207]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI [L106]</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -11192,10 +11202,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L107]
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [L106]</t>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
     </row>
@@ -11205,14 +11214,16 @@
           <t>14:30-15:30</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>CS161 (Problem Solving) Sem 1 (Pre-Mid) | DSAI [L207]
+CS161 (Problem Solving) Sem 1 (Post-Mid) | DSAI [L106]</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [C003]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [L404]</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -11225,10 +11236,9 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="F6" s="5" t="inlineStr">
-        <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L107]
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [L106]</t>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
     </row>
@@ -11253,9 +11263,10 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E7" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L208]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [L106]</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
@@ -11270,10 +11281,9 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="B8" s="5" t="inlineStr">
-        <is>
-          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [C305]
-CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [C002]</t>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Available - Free</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -11286,9 +11296,10 @@
           <t>Available - Free</t>
         </is>
       </c>
-      <c r="E8" s="4" t="inlineStr">
-        <is>
-          <t>Available - Free</t>
+      <c r="E8" s="5" t="inlineStr">
+        <is>
+          <t>CS303 (Computer Networks) Sem 5 (Pre-Mid) | CSE Sec A [L208]
+CS303 (Computer Networks) Sem 5 (Post-Mid) | CSE Sec A [L106]</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -11743,14 +11754,14 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [L106]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [L206]</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [L404]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [L407]</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -11878,8 +11889,8 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [L107]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [L207]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [L106]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -11911,8 +11922,8 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [L107]
-CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [L208]</t>
+          <t>CS262 (Software design tool and tecnique) Sem 3 (Pre-Mid) | CSE Sec B [L207]
+CS262 (Software design tool and tecnique) Sem 3 (Post-Mid) | CSE Sec B [L106]</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -11974,7 +11985,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11982,21 +11993,221 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="60" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>Status</t>
+          <t>Faculty</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Day</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Time Slot</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Details</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>No conflicts detected - All faculty schedules comply with availability</t>
-        </is>
+          <t>Sunil C K</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>Mon</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>10:30-12:00</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>DOUBLE-BOOKED (Pre-Mid): Teaching multiple courses simultaneously</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>Courses: CS309, CS161</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Sunil C K</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>Mon</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>10:30-12:00</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>DOUBLE-BOOKED (Post-Mid): Teaching multiple courses simultaneously</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>Courses: CS309, CS161</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Sunil P V</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>DOUBLE-BOOKED (Pre-Mid): Teaching multiple courses simultaneously</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>Courses: CS262, CS161</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Sunil P V</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>DOUBLE-BOOKED (Post-Mid): Teaching multiple courses simultaneously</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>Courses: CS262, CS161</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="35" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Total Conflicts</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Double-Booking (Multiple Courses)</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Scheduled on Unavailable Day</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Scheduled During Blocked Time</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -12135,8 +12346,8 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>HS152 (Economics/IET) Sem 1 (Pre-Mid) | ECE [C104]
-HS152 (Economics/IET) Sem 1 (Post-Mid) | ECE [C102]</t>
+          <t>HS152 (Economics/IET) Sem 1 (Pre-Mid) | ECE [C202]
+HS152 (Economics/IET) Sem 1 (Post-Mid) | ECE [C204]</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -12227,8 +12438,8 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>HS152 (Economics/IET) Sem 1 (Pre-Mid) | ECE [C104]
-HS152 (Economics/IET) Sem 1 (Post-Mid) | ECE [C202]</t>
+          <t>HS152 (Economics/IET) Sem 1 (Pre-Mid) | ECE [C302]
+HS152 (Economics/IET) Sem 1 (Post-Mid) | ECE [C205]</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -13282,8 +13493,8 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="54" customWidth="1" min="3" max="3"/>
-    <col width="54" customWidth="1" min="4" max="4"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
@@ -13370,8 +13581,8 @@
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>HS351 (Happiness &amp; Wellbeing) Sem 5 (Pre-Mid) | ECE
-HS351 (Happiness &amp; Wellbeing) Sem 5 (Post-Mid) | ECE</t>
+          <t>HS351 (Happiness &amp; Wellbeing) Sem 5 (Pre-Mid) | ECE [L404]
+HS351 (Happiness &amp; Wellbeing) Sem 5 (Post-Mid) | ECE [L404]</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -13494,8 +13705,8 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>HS351 (Happiness &amp; Wellbeing) Sem 5 (Pre-Mid) | ECE
-HS351 (Happiness &amp; Wellbeing) Sem 5 (Post-Mid) | ECE</t>
+          <t>HS351 (Happiness &amp; Wellbeing) Sem 5 (Pre-Mid) | ECE [L404]
+HS351 (Happiness &amp; Wellbeing) Sem 5 (Post-Mid) | ECE [L404]</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">

</xml_diff>